<commit_message>
metacritic research added to background
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C290DC8-5880-4165-8B06-C8543FD99F3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056F0753-C5E4-4037-AFFE-C9C3F3D5B996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Did my research on how Metacritic works, found some interesting things</t>
+  </si>
+  <si>
+    <t>Continuation on work for "Backgrounds and Methods"</t>
   </si>
 </sst>
 </file>
@@ -899,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +928,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -985,6 +988,17 @@
         <v>9</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43452</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished intro for background
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056F0753-C5E4-4037-AFFE-C9C3F3D5B996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194733FA-5766-4393-83B7-D73EDC07F233}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Continuation on work for "Backgrounds and Methods"</t>
+  </si>
+  <si>
+    <t>Some more work on "Background and Methodologies"</t>
   </si>
 </sst>
 </file>
@@ -902,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +931,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,6 +1003,14 @@
       </c>
       <c r="C8">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reading for background section
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194733FA-5766-4393-83B7-D73EDC07F233}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C42760-CF6E-4FD8-8E3A-C4C938FADC38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Some more work on "Background and Methodologies"</t>
+  </si>
+  <si>
+    <t>Read some of the potential "background"-section-related papers, wrote summaries for them. May need more material to read on.</t>
   </si>
 </sst>
 </file>
@@ -905,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +934,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,6 +1014,17 @@
       </c>
       <c r="C9">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43453</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished "background and methodologies"
Unless I need to revise it
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FF48C2-EB0D-4F57-92F2-6AEB36C24878}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4843F2-3BEA-468D-B4AF-CCBA6D6C773F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Looked, unsuccessfully, for some more sources to read on. Finished "background" section</t>
+  </si>
+  <si>
+    <t>Tackled the methodologies section</t>
   </si>
 </sst>
 </file>
@@ -911,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +940,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>9.8000000000000007</v>
+        <v>10.55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,6 +1039,14 @@
       </c>
       <c r="C11">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on data analysis
did some research on linear regression and started some actual work on data analysis
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CF36CA-84D4-4C25-89F1-73F12234FA2C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B44A6-A641-49A0-A627-C65B5D638C5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Started working on data analysis, not much though</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear regression research + work on data analysis </t>
   </si>
 </sst>
 </file>
@@ -917,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +946,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,6 +1064,17 @@
       </c>
       <c r="C13">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43456</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started to revise DA, questions 2 & 3
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB592424-8BC9-48DD-9EFF-45FF6F17E09D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7974D491-BD28-4B58-BCC8-0DC5972C3F66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Question 3 handled</t>
+  </si>
+  <si>
+    <t>Contemplation on how to approach what I have left</t>
+  </si>
+  <si>
+    <t>Started to rework questions 2 and 3 for Data Analysis. Looked into how to deal with outliers + things about linear regression.</t>
   </si>
 </sst>
 </file>
@@ -929,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +961,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>15.3</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,12 +1108,31 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43457</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tackling the outliers problem
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7974D491-BD28-4B58-BCC8-0DC5972C3F66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E45739C-F231-44DA-9E02-CE9F8F7F9A53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Started to rework questions 2 and 3 for Data Analysis. Looked into how to deal with outliers + things about linear regression.</t>
+  </si>
+  <si>
+    <t>Tackling the outliers problems + continuing with regression analysis</t>
   </si>
 </sst>
 </file>
@@ -935,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +964,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>16.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,6 +1135,14 @@
         <v>21</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
short summaries for time-management sources
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C98295-CB62-45F8-9076-B608134D13E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153CC8D9-C042-4125-9DE5-86F3F04F855B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Some more reading on time management, will try to tackle it today</t>
+  </si>
+  <si>
+    <t>Short summaries from my sources, to help out with the writing of time-management paper</t>
   </si>
 </sst>
 </file>
@@ -947,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +976,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>19.8</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,6 +1185,17 @@
         <v>25</v>
       </c>
       <c r="C23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43475</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
steam and steam spy info
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timon &amp; Pumba\Desktop\DwD-Individual-Project\Logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B646145-42F1-4DD2-9310-3736F48EC115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEF621D-2945-4B7C-ABFB-5663E17F1EDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Some small changes to Background and Methodologies</t>
+  </si>
+  <si>
+    <t>Steam and Steam Spy info</t>
   </si>
 </sst>
 </file>
@@ -962,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +991,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,6 +1250,17 @@
       </c>
       <c r="C28">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43489</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Background section is finished
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEF621D-2945-4B7C-ABFB-5663E17F1EDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C0B04-B9D8-4F84-B994-F6D0482A5B18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Steam and Steam Spy info</t>
+  </si>
+  <si>
+    <t>Finished updating Backgrounds section</t>
   </si>
 </sst>
 </file>
@@ -965,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +994,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,6 +1264,14 @@
       </c>
       <c r="C29">
         <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished Background and Methodologies
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C0B04-B9D8-4F84-B994-F6D0482A5B18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520224B-0F69-4EDF-B8D9-93DBCB1FD321}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Finished updating Backgrounds section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated the Methodologies section </t>
   </si>
 </sst>
 </file>
@@ -968,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +997,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>26.5</v>
+        <v>28.25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,6 +1275,17 @@
       </c>
       <c r="C30">
         <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43490</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
questions 2 & 3
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520224B-0F69-4EDF-B8D9-93DBCB1FD321}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46296807-5797-4E23-9DEE-698DD04C892F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">Updated the Methodologies section </t>
+  </si>
+  <si>
+    <t>Tackled questions 2 &amp; 3 from data analysis</t>
   </si>
 </sst>
 </file>
@@ -971,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1000,7 @@
       </c>
       <c r="F1">
         <f>SUM(C2:C32)</f>
-        <v>28.25</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1286,6 +1289,14 @@
       </c>
       <c r="C31">
         <v>1.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress on final paper
</commit_message>
<xml_diff>
--- a/Logs/work_logs.xlsx
+++ b/Logs/work_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMMonster\Desktop\DwD-Individual-Project\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359683DB-6AE7-49C3-B170-2E2C737D575A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EDD2A2-11DB-4228-84F7-AB600F8EAE66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Did question 1 to the best ability at the time, might need to revisit it if I'll have enough time/power (data analysis did ended up not too sophisticated in statistical sense)</t>
+  </si>
+  <si>
+    <t>Composed the final paper</t>
   </si>
 </sst>
 </file>
@@ -977,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,6 +1313,14 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>